<commit_message>
Reviewed inputs, outputs, and categories
Identified inputs and outputs from the interface.  Modified some
proposed names.  Added some categories
</commit_message>
<xml_diff>
--- a/testing/Variables with types.xlsx
+++ b/testing/Variables with types.xlsx
@@ -9,16 +9,17 @@
   <sheets>
     <sheet name="Variables with types" sheetId="1" r:id="rId1"/>
     <sheet name="Abbreviations" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Variables with types'!$C$1:$C$4204</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Variables with types'!$A$1:$I$4204</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12912" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12960" uniqueCount="427">
   <si>
     <t>A_Global</t>
   </si>
@@ -1030,9 +1031,6 @@
     <t>Near_Pristine_Land</t>
   </si>
   <si>
-    <t>Builtup</t>
-  </si>
-  <si>
     <t>kg_forage_per_kg_finished_product</t>
   </si>
   <si>
@@ -1288,9 +1286,6 @@
     <t>AP_target_stock_adj</t>
   </si>
   <si>
-    <t>non-productive land</t>
-  </si>
-  <si>
     <t>NO (import &amp; impact are both spelled out elsewhere)</t>
   </si>
   <si>
@@ -1298,6 +1293,91 @@
   </si>
   <si>
     <t>Use this abbreviation?</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>AP_demand_mod_pct</t>
+  </si>
+  <si>
+    <t>biofuel_mod_pct</t>
+  </si>
+  <si>
+    <t>CP_demand_mod_pct</t>
+  </si>
+  <si>
+    <t>CP_yield_mod_pct</t>
+  </si>
+  <si>
+    <t>forage_yield_mod_pct</t>
+  </si>
+  <si>
+    <t>other_demand_mod_pct</t>
+  </si>
+  <si>
+    <t>other_yield_mod_pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">global v country </t>
+  </si>
+  <si>
+    <t>near pristine land</t>
+  </si>
+  <si>
+    <t>Total_Crop_Land_Allocated_To_All_Other_Uses</t>
+  </si>
+  <si>
+    <r>
+      <t>Total_Crop_Land_Allocated_To_Commod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ties</t>
+    </r>
+  </si>
+  <si>
+    <t>shortfall</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>Forage_Prodn</t>
+  </si>
+  <si>
+    <t>requd_AP_prodn</t>
   </si>
 </sst>
 </file>
@@ -2126,10 +2206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4204"/>
+  <dimension ref="A1:I4204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="D290" sqref="D290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,7 +2219,7 @@
     <col min="4" max="4" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>288</v>
       </c>
@@ -2161,8 +2241,14 @@
       <c r="G1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>406</v>
+      </c>
+      <c r="I1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2172,11 +2258,14 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
       <c r="G2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2187,13 +2276,13 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2203,11 +2292,17 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>408</v>
+      </c>
       <c r="G4" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2218,10 +2313,13 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+      <c r="F5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2235,7 +2333,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2246,13 +2344,13 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G7" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2262,14 +2360,20 @@
       <c r="C8" t="s">
         <v>2</v>
       </c>
+      <c r="D8" t="s">
+        <v>409</v>
+      </c>
       <c r="E8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G8" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2280,13 +2384,13 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="G9" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2297,13 +2401,13 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E10" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2314,13 +2418,13 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G11" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2331,7 +2435,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F12" t="s">
         <v>296</v>
@@ -2340,7 +2444,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2350,14 +2454,20 @@
       <c r="C13" t="s">
         <v>2</v>
       </c>
+      <c r="D13" t="s">
+        <v>410</v>
+      </c>
       <c r="F13" t="s">
         <v>297</v>
       </c>
       <c r="G13" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2371,7 +2481,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2381,11 +2491,17 @@
       <c r="C15" t="s">
         <v>2</v>
       </c>
+      <c r="D15" t="s">
+        <v>411</v>
+      </c>
       <c r="G15" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2395,11 +2511,14 @@
       <c r="C16" t="s">
         <v>2</v>
       </c>
+      <c r="D16" t="s">
+        <v>130</v>
+      </c>
       <c r="G16" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2416,7 +2535,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -2426,14 +2545,20 @@
       <c r="C18" t="s">
         <v>2</v>
       </c>
+      <c r="D18" t="s">
+        <v>412</v>
+      </c>
       <c r="F18" t="s">
         <v>299</v>
       </c>
       <c r="G18" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2444,13 +2569,16 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="F19" t="s">
+        <v>303</v>
       </c>
       <c r="G19" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2467,7 +2595,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2481,10 +2609,13 @@
         <v>301</v>
       </c>
       <c r="E21" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+      <c r="F21" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2497,8 +2628,11 @@
       <c r="D22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2512,7 +2646,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2523,7 +2657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2533,11 +2667,14 @@
       <c r="C25" t="s">
         <v>2</v>
       </c>
+      <c r="D25" t="s">
+        <v>320</v>
+      </c>
       <c r="G25" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2547,11 +2684,14 @@
       <c r="C26" t="s">
         <v>2</v>
       </c>
+      <c r="D26" t="s">
+        <v>321</v>
+      </c>
       <c r="E26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2565,7 +2705,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2575,11 +2715,17 @@
       <c r="C28" t="s">
         <v>2</v>
       </c>
+      <c r="D28" t="s">
+        <v>413</v>
+      </c>
       <c r="G28" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2593,7 +2739,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -2603,11 +2749,17 @@
       <c r="C30" t="s">
         <v>2</v>
       </c>
+      <c r="D30" t="s">
+        <v>414</v>
+      </c>
       <c r="G30" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2623,8 +2775,11 @@
       <c r="G31" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +2793,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2648,11 +2803,14 @@
       <c r="C33" t="s">
         <v>2</v>
       </c>
+      <c r="D33" t="s">
+        <v>251</v>
+      </c>
       <c r="G33" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2663,13 +2821,13 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
+        <v>340</v>
+      </c>
+      <c r="E34" t="s">
         <v>341</v>
       </c>
-      <c r="E34" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2680,13 +2838,13 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E35" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -2696,8 +2854,11 @@
       <c r="C36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2707,8 +2868,11 @@
       <c r="C37" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -2718,8 +2882,11 @@
       <c r="C38" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -2729,8 +2896,11 @@
       <c r="C39" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -2741,7 +2911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2752,7 +2922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -2763,7 +2933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -2774,7 +2944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -2785,7 +2955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -2795,8 +2965,11 @@
       <c r="C45" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2810,7 +2983,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2821,7 +2994,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2832,7 +3005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -2843,7 +3016,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -2854,7 +3027,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -2864,8 +3037,11 @@
       <c r="C51" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -2876,10 +3052,16 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+      <c r="F52" t="s">
+        <v>383</v>
+      </c>
+      <c r="I52" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -2890,7 +3072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -2900,8 +3082,11 @@
       <c r="C54" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>46</v>
       </c>
@@ -2912,10 +3097,10 @@
         <v>51</v>
       </c>
       <c r="E55" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>46</v>
       </c>
@@ -2926,7 +3111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -2937,10 +3122,10 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>46</v>
       </c>
@@ -2951,10 +3136,10 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>46</v>
       </c>
@@ -2968,7 +3153,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>46</v>
       </c>
@@ -2982,7 +3167,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>46</v>
       </c>
@@ -2993,7 +3178,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>46</v>
       </c>
@@ -3004,7 +3189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>46</v>
       </c>
@@ -3018,7 +3203,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>46</v>
       </c>
@@ -3032,10 +3217,10 @@
         <v>304</v>
       </c>
       <c r="E64" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -3049,7 +3234,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>46</v>
       </c>
@@ -3060,7 +3245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -3071,7 +3256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>46</v>
       </c>
@@ -3085,7 +3270,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>46</v>
       </c>
@@ -3096,7 +3281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>46</v>
       </c>
@@ -3107,7 +3292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>46</v>
       </c>
@@ -3121,7 +3306,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>46</v>
       </c>
@@ -3132,7 +3317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>46</v>
       </c>
@@ -3143,7 +3328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>46</v>
       </c>
@@ -3154,7 +3339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>46</v>
       </c>
@@ -3165,10 +3350,10 @@
         <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>46</v>
       </c>
@@ -3179,7 +3364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>46</v>
       </c>
@@ -3190,7 +3375,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>46</v>
       </c>
@@ -3201,7 +3386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>46</v>
       </c>
@@ -3212,7 +3397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>46</v>
       </c>
@@ -3224,6 +3409,9 @@
       </c>
       <c r="D80" t="s">
         <v>308</v>
+      </c>
+      <c r="I80" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3279,7 +3467,7 @@
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E84" t="s">
         <v>2</v>
@@ -3313,7 +3501,7 @@
         <v>310</v>
       </c>
       <c r="E86" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3327,7 +3515,7 @@
         <v>12</v>
       </c>
       <c r="D87" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E87" t="s">
         <v>311</v>
@@ -3358,7 +3546,7 @@
         <v>12</v>
       </c>
       <c r="E89" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G89" t="s">
         <v>313</v>
@@ -3541,7 +3729,7 @@
         <v>51</v>
       </c>
       <c r="D104" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3555,7 +3743,7 @@
         <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3568,6 +3756,9 @@
       <c r="C106" t="s">
         <v>2</v>
       </c>
+      <c r="F106" t="s">
+        <v>381</v>
+      </c>
       <c r="G106" t="s">
         <v>313</v>
       </c>
@@ -3608,7 +3799,7 @@
         <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3622,7 +3813,7 @@
         <v>2</v>
       </c>
       <c r="E110" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3650,7 +3841,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>46</v>
       </c>
@@ -3664,7 +3855,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>46</v>
       </c>
@@ -3678,10 +3869,10 @@
         <v>314</v>
       </c>
       <c r="E114" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>46</v>
       </c>
@@ -3695,7 +3886,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>46</v>
       </c>
@@ -3709,7 +3900,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>46</v>
       </c>
@@ -3720,7 +3911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>46</v>
       </c>
@@ -3731,10 +3922,10 @@
         <v>2</v>
       </c>
       <c r="E118" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>46</v>
       </c>
@@ -3745,13 +3936,13 @@
         <v>2</v>
       </c>
       <c r="E119" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G119" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>46</v>
       </c>
@@ -3764,8 +3955,11 @@
       <c r="G120" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I120" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>46</v>
       </c>
@@ -3779,7 +3973,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>46</v>
       </c>
@@ -3793,7 +3987,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>46</v>
       </c>
@@ -3804,13 +3998,13 @@
         <v>2</v>
       </c>
       <c r="E123" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G123" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>46</v>
       </c>
@@ -3821,7 +4015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>46</v>
       </c>
@@ -3832,7 +4026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>46</v>
       </c>
@@ -3846,7 +4040,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>46</v>
       </c>
@@ -3860,7 +4054,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>46</v>
       </c>
@@ -3882,7 +4076,7 @@
         <v>2</v>
       </c>
       <c r="D129" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G129" t="s">
         <v>313</v>
@@ -3913,7 +4107,7 @@
         <v>316</v>
       </c>
       <c r="E131" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -3952,7 +4146,7 @@
         <v>2</v>
       </c>
       <c r="E134" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4088,7 +4282,7 @@
         <v>2</v>
       </c>
       <c r="E145" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -4126,6 +4320,9 @@
       <c r="C148" t="s">
         <v>2</v>
       </c>
+      <c r="D148" t="s">
+        <v>425</v>
+      </c>
       <c r="G148" t="s">
         <v>313</v>
       </c>
@@ -4163,7 +4360,7 @@
         <v>2</v>
       </c>
       <c r="E151" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G151" t="s">
         <v>313</v>
@@ -4191,7 +4388,7 @@
         <v>2</v>
       </c>
       <c r="D153" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G153" t="s">
         <v>313</v>
@@ -4236,7 +4433,7 @@
         <v>2</v>
       </c>
       <c r="E156" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -4289,7 +4486,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>46</v>
       </c>
@@ -4303,7 +4500,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>46</v>
       </c>
@@ -4314,10 +4511,10 @@
         <v>2</v>
       </c>
       <c r="E162" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>46</v>
       </c>
@@ -4328,10 +4525,10 @@
         <v>2</v>
       </c>
       <c r="D163" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>46</v>
       </c>
@@ -4342,10 +4539,10 @@
         <v>2</v>
       </c>
       <c r="E164" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>46</v>
       </c>
@@ -4356,7 +4553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>46</v>
       </c>
@@ -4367,10 +4564,10 @@
         <v>2</v>
       </c>
       <c r="E166" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>46</v>
       </c>
@@ -4381,10 +4578,10 @@
         <v>2</v>
       </c>
       <c r="D167" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>46</v>
       </c>
@@ -4395,7 +4592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>46</v>
       </c>
@@ -4408,8 +4605,11 @@
       <c r="D169" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I169" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>46</v>
       </c>
@@ -4420,7 +4620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>46</v>
       </c>
@@ -4431,7 +4631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>46</v>
       </c>
@@ -4445,7 +4645,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>46</v>
       </c>
@@ -4456,10 +4656,10 @@
         <v>51</v>
       </c>
       <c r="D173" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>46</v>
       </c>
@@ -4470,10 +4670,10 @@
         <v>2</v>
       </c>
       <c r="D174" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>46</v>
       </c>
@@ -4487,7 +4687,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>46</v>
       </c>
@@ -4498,7 +4698,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>46</v>
       </c>
@@ -4509,7 +4709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>46</v>
       </c>
@@ -4520,7 +4720,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>46</v>
       </c>
@@ -4531,7 +4731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>46</v>
       </c>
@@ -4542,7 +4742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>46</v>
       </c>
@@ -4553,7 +4753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>46</v>
       </c>
@@ -4567,7 +4767,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>46</v>
       </c>
@@ -4581,7 +4781,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>46</v>
       </c>
@@ -4595,7 +4795,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>46</v>
       </c>
@@ -4608,8 +4808,11 @@
       <c r="D185" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I185" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>46</v>
       </c>
@@ -4620,7 +4823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>46</v>
       </c>
@@ -4631,7 +4834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>46</v>
       </c>
@@ -4642,7 +4845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>46</v>
       </c>
@@ -4653,7 +4856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>46</v>
       </c>
@@ -4664,7 +4867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>46</v>
       </c>
@@ -4675,7 +4878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>46</v>
       </c>
@@ -4875,10 +5078,10 @@
         <v>2</v>
       </c>
       <c r="D207" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E207" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G207" t="s">
         <v>313</v>
@@ -5069,7 +5272,7 @@
         <v>2</v>
       </c>
       <c r="D223" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -5097,7 +5300,7 @@
         <v>2</v>
       </c>
       <c r="D225" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -5111,7 +5314,7 @@
         <v>2</v>
       </c>
       <c r="D226" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -5124,6 +5327,9 @@
       <c r="C227" t="s">
         <v>2</v>
       </c>
+      <c r="D227" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
@@ -5172,7 +5378,7 @@
         <v>2</v>
       </c>
       <c r="D231" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -5208,7 +5414,7 @@
         <v>2</v>
       </c>
       <c r="D234" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
@@ -5222,7 +5428,7 @@
         <v>2</v>
       </c>
       <c r="D235" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
@@ -5289,7 +5495,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>46</v>
       </c>
@@ -5300,10 +5506,10 @@
         <v>2</v>
       </c>
       <c r="D241" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>46</v>
       </c>
@@ -5314,7 +5520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>46</v>
       </c>
@@ -5325,7 +5531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>46</v>
       </c>
@@ -5336,7 +5542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>46</v>
       </c>
@@ -5347,7 +5553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>46</v>
       </c>
@@ -5357,8 +5563,11 @@
       <c r="C246" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I246" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>46</v>
       </c>
@@ -5372,7 +5581,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>46</v>
       </c>
@@ -5383,7 +5592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>46</v>
       </c>
@@ -5394,7 +5603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>46</v>
       </c>
@@ -5405,7 +5614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>46</v>
       </c>
@@ -5419,7 +5628,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>46</v>
       </c>
@@ -5429,8 +5638,14 @@
       <c r="C252" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D252" t="s">
+        <v>417</v>
+      </c>
+      <c r="I252" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>46</v>
       </c>
@@ -5440,8 +5655,11 @@
       <c r="C253" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D253" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>46</v>
       </c>
@@ -5452,7 +5670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>46</v>
       </c>
@@ -5463,7 +5681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>46</v>
       </c>
@@ -5474,7 +5692,7 @@
         <v>2</v>
       </c>
       <c r="D256" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -5488,7 +5706,7 @@
         <v>2</v>
       </c>
       <c r="D257" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -48909,12 +49127,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C4204"/>
+  <autoFilter ref="A1:I4204"/>
   <sortState ref="A2:G4204">
     <sortCondition ref="A2:A4204"/>
     <sortCondition ref="B2:B4204"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -48923,7 +49142,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48937,27 +49156,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B1" t="s">
         <v>369</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D1" t="s">
         <v>370</v>
       </c>
-      <c r="C1" t="s">
-        <v>407</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>371</v>
-      </c>
-      <c r="E1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -48968,10 +49187,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -48982,7 +49201,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -48993,10 +49212,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -49007,10 +49226,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -49021,10 +49240,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -49035,10 +49254,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -49049,10 +49268,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -49066,7 +49285,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>404</v>
+        <v>416</v>
+      </c>
+      <c r="C10" t="s">
+        <v>395</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -49077,10 +49299,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C11" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -49091,10 +49313,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -49105,10 +49327,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -49119,10 +49341,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -49133,10 +49355,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
@@ -49147,13 +49369,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
@@ -49178,10 +49400,10 @@
         <v>311</v>
       </c>
       <c r="B18" t="s">
+        <v>394</v>
+      </c>
+      <c r="C18" t="s">
         <v>395</v>
-      </c>
-      <c r="C18" t="s">
-        <v>396</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
@@ -49192,7 +49414,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D19" t="s">
         <v>46</v>
@@ -49203,10 +49425,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B20" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -49217,13 +49439,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -49234,10 +49456,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D22" t="s">
         <v>46</v>
@@ -49248,10 +49470,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B23" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D23" t="s">
         <v>46</v>
@@ -49262,10 +49484,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
@@ -49276,7 +49498,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D25" t="s">
         <v>46</v>
@@ -49287,10 +49509,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D26" t="s">
         <v>46</v>
@@ -49301,10 +49523,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C27" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D27" t="s">
         <v>46</v>
@@ -49315,10 +49537,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D28" t="s">
         <v>46</v>
@@ -49329,10 +49551,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D29" t="s">
         <v>46</v>
@@ -49343,10 +49565,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>385</v>
+      </c>
+      <c r="B30" t="s">
         <v>386</v>
-      </c>
-      <c r="B30" t="s">
-        <v>387</v>
       </c>
       <c r="D30" t="s">
         <v>46</v>
@@ -49357,19 +49579,37 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B31" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C31" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D31" t="s">
         <v>46</v>
       </c>
       <c r="E31" t="s">
         <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added proposed variable changes in response to issues #6 and #8
</commit_message>
<xml_diff>
--- a/testing/Variables with types.xlsx
+++ b/testing/Variables with types.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12960" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13019" uniqueCount="485">
   <si>
     <t>A_Global</t>
   </si>
@@ -1172,9 +1172,6 @@
     <t>commodity_prodn</t>
   </si>
   <si>
-    <t>Crop_land_data</t>
-  </si>
-  <si>
     <t>press</t>
   </si>
   <si>
@@ -1271,9 +1268,6 @@
     <t>reqd_chg_commodity_inventory</t>
   </si>
   <si>
-    <t>c_inventory_impact_on_consn</t>
-  </si>
-  <si>
     <t>chg_indicated_land_alloc</t>
   </si>
   <si>
@@ -1328,34 +1322,6 @@
     <t>near pristine land</t>
   </si>
   <si>
-    <t>Total_Crop_Land_Allocated_To_All_Other_Uses</t>
-  </si>
-  <si>
-    <r>
-      <t>Total_Crop_Land_Allocated_To_Commod</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ties</t>
-    </r>
-  </si>
-  <si>
     <t>shortfall</t>
   </si>
   <si>
@@ -1374,10 +1340,196 @@
     <t>import</t>
   </si>
   <si>
-    <t>Forage_Prodn</t>
+    <t>AP_demand_mod_logic</t>
   </si>
   <si>
-    <t>requd_AP_prodn</t>
+    <t>biofuel_mod_logic</t>
+  </si>
+  <si>
+    <t>CP_demand_mod_logic</t>
+  </si>
+  <si>
+    <t>CP_yield_mod_logic</t>
+  </si>
+  <si>
+    <t>forage_yield_mod_logic</t>
+  </si>
+  <si>
+    <t>GDP_mod_pct</t>
+  </si>
+  <si>
+    <t>GDP_mod_logic</t>
+  </si>
+  <si>
+    <t>other_demand_mod_logic</t>
+  </si>
+  <si>
+    <t>other_yield_mod_logic</t>
+  </si>
+  <si>
+    <t>population_mod_logic</t>
+  </si>
+  <si>
+    <t>population_mod_pct</t>
+  </si>
+  <si>
+    <t>abandoned_land_data</t>
+  </si>
+  <si>
+    <t>AP_export_averaging_time</t>
+  </si>
+  <si>
+    <t>AP_exports</t>
+  </si>
+  <si>
+    <t>AP_imports</t>
+  </si>
+  <si>
+    <t>builtup_land_data</t>
+  </si>
+  <si>
+    <t>chg_net_AP_export</t>
+  </si>
+  <si>
+    <t>CP_inventory_impact_on_consn</t>
+  </si>
+  <si>
+    <t>CP_export_averaging_time</t>
+  </si>
+  <si>
+    <t>CP_inventory_ratio</t>
+  </si>
+  <si>
+    <t>chg_net_CP_export</t>
+  </si>
+  <si>
+    <t>commodity_disposition_data_other</t>
+  </si>
+  <si>
+    <t>CP_crosswalk</t>
+  </si>
+  <si>
+    <t>CP_crosswalk_input</t>
+  </si>
+  <si>
+    <t>CP_protein_mass_crosswalk</t>
+  </si>
+  <si>
+    <t>crop_land_alloc_to_cellulosic_energy_crop</t>
+  </si>
+  <si>
+    <t>crop_land_alloc_to_fallow</t>
+  </si>
+  <si>
+    <t>crop_land_alloc_to_fiber</t>
+  </si>
+  <si>
+    <t>crop_land_alloc_to_other</t>
+  </si>
+  <si>
+    <t>crop_land_alloc_to_VFN</t>
+  </si>
+  <si>
+    <t>commodity_disposition_data_fiber</t>
+  </si>
+  <si>
+    <t>crop_to_latent</t>
+  </si>
+  <si>
+    <t>crop_land_data</t>
+  </si>
+  <si>
+    <t>exports</t>
+  </si>
+  <si>
+    <t>F_crosswalk_input</t>
+  </si>
+  <si>
+    <t>F_protein_mass_crosswalk</t>
+  </si>
+  <si>
+    <t>forage_prodn</t>
+  </si>
+  <si>
+    <t>forest_frac</t>
+  </si>
+  <si>
+    <t>GDP_per_capita</t>
+  </si>
+  <si>
+    <t>GDP_per_capita_scenario</t>
+  </si>
+  <si>
+    <t>imports</t>
+  </si>
+  <si>
+    <t>indicated_land_alloc</t>
+  </si>
+  <si>
+    <t>indicated_NPL</t>
+  </si>
+  <si>
+    <t>latent_land_data</t>
+  </si>
+  <si>
+    <t>latent_to_crop</t>
+  </si>
+  <si>
+    <t>max_NPL_forest</t>
+  </si>
+  <si>
+    <t>milling_factor_fiber</t>
+  </si>
+  <si>
+    <t>milling_factor_other</t>
+  </si>
+  <si>
+    <t>NPL_data</t>
+  </si>
+  <si>
+    <t>other_area_harvested_data</t>
+  </si>
+  <si>
+    <t>other_yield</t>
+  </si>
+  <si>
+    <t>per_capita_fiber_demand_scenario</t>
+  </si>
+  <si>
+    <t>per_capita_other_consn</t>
+  </si>
+  <si>
+    <t>per_capita_fiber_consn</t>
+  </si>
+  <si>
+    <t>per_capita_VFN_demand_scenario</t>
+  </si>
+  <si>
+    <t>per_capita_other_demand_scenario</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>reqd_AP_commodity_consn_2D</t>
+  </si>
+  <si>
+    <t>reqd_AP_prodn</t>
+  </si>
+  <si>
+    <t>reqd_built_up_land</t>
+  </si>
+  <si>
+    <t>reqd_fiber_prodn</t>
+  </si>
+  <si>
+    <t>reqd_other_prodn</t>
+  </si>
+  <si>
+    <t>set_aside_land_data</t>
+  </si>
+  <si>
+    <t>total_AP_prodn_shortfall</t>
   </si>
 </sst>
 </file>
@@ -2208,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D290" sqref="D290"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2242,10 +2394,10 @@
         <v>294</v>
       </c>
       <c r="H1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2275,6 +2427,9 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>421</v>
+      </c>
       <c r="E3" t="s">
         <v>331</v>
       </c>
@@ -2293,7 +2448,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G4" t="s">
         <v>313</v>
@@ -2312,11 +2467,14 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
       <c r="E5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2343,6 +2501,9 @@
       <c r="C7" t="s">
         <v>2</v>
       </c>
+      <c r="D7" t="s">
+        <v>422</v>
+      </c>
       <c r="E7" t="s">
         <v>356</v>
       </c>
@@ -2361,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E8" t="s">
         <v>334</v>
@@ -2434,6 +2595,9 @@
       <c r="C12" t="s">
         <v>2</v>
       </c>
+      <c r="D12" t="s">
+        <v>423</v>
+      </c>
       <c r="E12" t="s">
         <v>336</v>
       </c>
@@ -2455,7 +2619,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F13" t="s">
         <v>297</v>
@@ -2477,6 +2641,9 @@
       <c r="C14" t="s">
         <v>2</v>
       </c>
+      <c r="D14" t="s">
+        <v>424</v>
+      </c>
       <c r="G14" t="s">
         <v>313</v>
       </c>
@@ -2492,7 +2659,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G15" t="s">
         <v>313</v>
@@ -2528,6 +2695,9 @@
       <c r="C17" t="s">
         <v>2</v>
       </c>
+      <c r="D17" t="s">
+        <v>425</v>
+      </c>
       <c r="F17" t="s">
         <v>298</v>
       </c>
@@ -2546,7 +2716,7 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F18" t="s">
         <v>299</v>
@@ -2568,6 +2738,9 @@
       <c r="C19" t="s">
         <v>2</v>
       </c>
+      <c r="D19" t="s">
+        <v>426</v>
+      </c>
       <c r="E19" t="s">
         <v>355</v>
       </c>
@@ -2588,6 +2761,9 @@
       <c r="C20" t="s">
         <v>2</v>
       </c>
+      <c r="D20" t="s">
+        <v>427</v>
+      </c>
       <c r="F20" t="s">
         <v>300</v>
       </c>
@@ -2612,7 +2788,7 @@
         <v>337</v>
       </c>
       <c r="F21" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2629,7 +2805,7 @@
         <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2701,6 +2877,9 @@
       <c r="C27" t="s">
         <v>2</v>
       </c>
+      <c r="D27" t="s">
+        <v>428</v>
+      </c>
       <c r="G27" t="s">
         <v>313</v>
       </c>
@@ -2716,7 +2895,7 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G28" t="s">
         <v>313</v>
@@ -2735,6 +2914,9 @@
       <c r="C29" t="s">
         <v>2</v>
       </c>
+      <c r="D29" t="s">
+        <v>429</v>
+      </c>
       <c r="G29" t="s">
         <v>313</v>
       </c>
@@ -2750,7 +2932,7 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G30" t="s">
         <v>313</v>
@@ -2769,6 +2951,9 @@
       <c r="C31" t="s">
         <v>2</v>
       </c>
+      <c r="D31" t="s">
+        <v>431</v>
+      </c>
       <c r="F31" t="s">
         <v>303</v>
       </c>
@@ -2789,6 +2974,9 @@
       <c r="C32" t="s">
         <v>2</v>
       </c>
+      <c r="D32" t="s">
+        <v>430</v>
+      </c>
       <c r="G32" t="s">
         <v>313</v>
       </c>
@@ -2855,7 +3043,7 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2869,7 +3057,7 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2883,7 +3071,7 @@
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2897,7 +3085,7 @@
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2979,6 +3167,9 @@
       <c r="C46" t="s">
         <v>2</v>
       </c>
+      <c r="D46" t="s">
+        <v>432</v>
+      </c>
       <c r="G46" t="s">
         <v>313</v>
       </c>
@@ -3055,7 +3246,7 @@
         <v>361</v>
       </c>
       <c r="F52" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I52" t="s">
         <v>313</v>
@@ -3083,7 +3274,7 @@
         <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3149,6 +3340,9 @@
       <c r="C59" t="s">
         <v>2</v>
       </c>
+      <c r="D59" t="s">
+        <v>433</v>
+      </c>
       <c r="G59" t="s">
         <v>313</v>
       </c>
@@ -3163,6 +3357,9 @@
       <c r="C60" t="s">
         <v>2</v>
       </c>
+      <c r="D60" t="s">
+        <v>434</v>
+      </c>
       <c r="G60" t="s">
         <v>313</v>
       </c>
@@ -3199,6 +3396,9 @@
       <c r="C63" t="s">
         <v>2</v>
       </c>
+      <c r="D63" t="s">
+        <v>435</v>
+      </c>
       <c r="G63" t="s">
         <v>313</v>
       </c>
@@ -3350,7 +3550,7 @@
         <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3438,6 +3638,9 @@
       <c r="C82" t="s">
         <v>2</v>
       </c>
+      <c r="D82" t="s">
+        <v>436</v>
+      </c>
       <c r="G82" t="s">
         <v>313</v>
       </c>
@@ -3452,6 +3655,9 @@
       <c r="C83" t="s">
         <v>2</v>
       </c>
+      <c r="D83" t="s">
+        <v>439</v>
+      </c>
       <c r="E83" t="s">
         <v>2</v>
       </c>
@@ -3467,7 +3673,7 @@
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>398</v>
+        <v>438</v>
       </c>
       <c r="E84" t="s">
         <v>2</v>
@@ -3483,6 +3689,9 @@
       <c r="C85" t="s">
         <v>2</v>
       </c>
+      <c r="D85" t="s">
+        <v>440</v>
+      </c>
       <c r="E85" t="s">
         <v>2</v>
       </c>
@@ -3515,7 +3724,7 @@
         <v>12</v>
       </c>
       <c r="D87" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E87" t="s">
         <v>311</v>
@@ -3531,6 +3740,9 @@
       <c r="C88" t="s">
         <v>12</v>
       </c>
+      <c r="D88" t="s">
+        <v>437</v>
+      </c>
       <c r="G88" t="s">
         <v>313</v>
       </c>
@@ -3545,6 +3757,9 @@
       <c r="C89" t="s">
         <v>12</v>
       </c>
+      <c r="D89" t="s">
+        <v>441</v>
+      </c>
       <c r="E89" t="s">
         <v>346</v>
       </c>
@@ -3631,6 +3846,9 @@
       <c r="C96" t="s">
         <v>2</v>
       </c>
+      <c r="D96" t="s">
+        <v>451</v>
+      </c>
       <c r="G96" t="s">
         <v>313</v>
       </c>
@@ -3645,6 +3863,9 @@
       <c r="C97" t="s">
         <v>2</v>
       </c>
+      <c r="D97" t="s">
+        <v>442</v>
+      </c>
       <c r="G97" t="s">
         <v>313</v>
       </c>
@@ -3743,7 +3964,7 @@
         <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3756,8 +3977,11 @@
       <c r="C106" t="s">
         <v>2</v>
       </c>
+      <c r="D106" t="s">
+        <v>443</v>
+      </c>
       <c r="F106" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G106" t="s">
         <v>313</v>
@@ -3784,6 +4008,9 @@
       <c r="C108" t="s">
         <v>2</v>
       </c>
+      <c r="D108" t="s">
+        <v>444</v>
+      </c>
       <c r="G108" t="s">
         <v>313</v>
       </c>
@@ -3851,6 +4078,9 @@
       <c r="C113" t="s">
         <v>2</v>
       </c>
+      <c r="D113" t="s">
+        <v>445</v>
+      </c>
       <c r="G113" t="s">
         <v>313</v>
       </c>
@@ -3935,6 +4165,9 @@
       <c r="C119" t="s">
         <v>2</v>
       </c>
+      <c r="D119" t="s">
+        <v>446</v>
+      </c>
       <c r="E119" t="s">
         <v>350</v>
       </c>
@@ -3952,6 +4185,9 @@
       <c r="C120" t="s">
         <v>2</v>
       </c>
+      <c r="D120" t="s">
+        <v>447</v>
+      </c>
       <c r="G120" t="s">
         <v>313</v>
       </c>
@@ -3969,6 +4205,9 @@
       <c r="C121" t="s">
         <v>2</v>
       </c>
+      <c r="D121" t="s">
+        <v>448</v>
+      </c>
       <c r="G121" t="s">
         <v>313</v>
       </c>
@@ -3983,6 +4222,9 @@
       <c r="C122" t="s">
         <v>2</v>
       </c>
+      <c r="D122" t="s">
+        <v>449</v>
+      </c>
       <c r="G122" t="s">
         <v>313</v>
       </c>
@@ -3997,6 +4239,9 @@
       <c r="C123" t="s">
         <v>2</v>
       </c>
+      <c r="D123" t="s">
+        <v>450</v>
+      </c>
       <c r="E123" t="s">
         <v>351</v>
       </c>
@@ -4064,6 +4309,9 @@
       <c r="C128" t="s">
         <v>51</v>
       </c>
+      <c r="D128" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
@@ -4076,7 +4324,7 @@
         <v>2</v>
       </c>
       <c r="D129" t="s">
-        <v>365</v>
+        <v>453</v>
       </c>
       <c r="G129" t="s">
         <v>313</v>
@@ -4134,6 +4382,9 @@
       <c r="C133" t="s">
         <v>2</v>
       </c>
+      <c r="D133" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
@@ -4170,6 +4421,9 @@
       <c r="C136" t="s">
         <v>2</v>
       </c>
+      <c r="D136" t="s">
+        <v>455</v>
+      </c>
       <c r="G136" t="s">
         <v>313</v>
       </c>
@@ -4184,6 +4438,9 @@
       <c r="C137" t="s">
         <v>2</v>
       </c>
+      <c r="D137" t="s">
+        <v>456</v>
+      </c>
       <c r="G137" t="s">
         <v>313</v>
       </c>
@@ -4321,7 +4578,7 @@
         <v>2</v>
       </c>
       <c r="D148" t="s">
-        <v>425</v>
+        <v>457</v>
       </c>
       <c r="G148" t="s">
         <v>313</v>
@@ -4359,6 +4616,9 @@
       <c r="C151" t="s">
         <v>2</v>
       </c>
+      <c r="D151" t="s">
+        <v>458</v>
+      </c>
       <c r="E151" t="s">
         <v>353</v>
       </c>
@@ -4404,6 +4664,9 @@
       <c r="C154" t="s">
         <v>2</v>
       </c>
+      <c r="D154" t="s">
+        <v>459</v>
+      </c>
       <c r="G154" t="s">
         <v>313</v>
       </c>
@@ -4418,6 +4681,9 @@
       <c r="C155" t="s">
         <v>2</v>
       </c>
+      <c r="D155" t="s">
+        <v>460</v>
+      </c>
       <c r="G155" t="s">
         <v>313</v>
       </c>
@@ -4446,6 +4712,9 @@
       <c r="C157" t="s">
         <v>2</v>
       </c>
+      <c r="D157" t="s">
+        <v>461</v>
+      </c>
       <c r="G157" t="s">
         <v>313</v>
       </c>
@@ -4482,6 +4751,9 @@
       <c r="C160" t="s">
         <v>6</v>
       </c>
+      <c r="D160" t="s">
+        <v>462</v>
+      </c>
       <c r="G160" t="s">
         <v>313</v>
       </c>
@@ -4496,6 +4768,9 @@
       <c r="C161" t="s">
         <v>2</v>
       </c>
+      <c r="D161" t="s">
+        <v>463</v>
+      </c>
       <c r="G161" t="s">
         <v>313</v>
       </c>
@@ -4641,6 +4916,9 @@
       <c r="C172" t="s">
         <v>2</v>
       </c>
+      <c r="D172" t="s">
+        <v>464</v>
+      </c>
       <c r="G172" t="s">
         <v>313</v>
       </c>
@@ -4683,6 +4961,9 @@
       <c r="C175" t="s">
         <v>51</v>
       </c>
+      <c r="D175" t="s">
+        <v>465</v>
+      </c>
       <c r="G175" t="s">
         <v>313</v>
       </c>
@@ -4741,6 +5022,9 @@
       <c r="C180" t="s">
         <v>2</v>
       </c>
+      <c r="D180" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
@@ -4763,6 +5047,9 @@
       <c r="C182" t="s">
         <v>2</v>
       </c>
+      <c r="D182" t="s">
+        <v>467</v>
+      </c>
       <c r="G182" t="s">
         <v>313</v>
       </c>
@@ -4777,6 +5064,9 @@
       <c r="C183" t="s">
         <v>2</v>
       </c>
+      <c r="D183" t="s">
+        <v>468</v>
+      </c>
       <c r="G183" t="s">
         <v>313</v>
       </c>
@@ -4888,6 +5178,9 @@
       <c r="C192" t="s">
         <v>2</v>
       </c>
+      <c r="D192" t="s">
+        <v>469</v>
+      </c>
       <c r="G192" t="s">
         <v>313</v>
       </c>
@@ -4935,6 +5228,9 @@
       <c r="C196" t="s">
         <v>2</v>
       </c>
+      <c r="D196" t="s">
+        <v>470</v>
+      </c>
       <c r="G196" t="s">
         <v>313</v>
       </c>
@@ -4949,6 +5245,9 @@
       <c r="C197" t="s">
         <v>2</v>
       </c>
+      <c r="D197" t="s">
+        <v>471</v>
+      </c>
       <c r="G197" t="s">
         <v>313</v>
       </c>
@@ -5007,6 +5306,9 @@
       <c r="C202" t="s">
         <v>2</v>
       </c>
+      <c r="D202" t="s">
+        <v>474</v>
+      </c>
       <c r="G202" t="s">
         <v>313</v>
       </c>
@@ -5021,6 +5323,9 @@
       <c r="C203" t="s">
         <v>2</v>
       </c>
+      <c r="D203" t="s">
+        <v>472</v>
+      </c>
       <c r="G203" t="s">
         <v>313</v>
       </c>
@@ -5035,6 +5340,9 @@
       <c r="C204" t="s">
         <v>2</v>
       </c>
+      <c r="D204" t="s">
+        <v>473</v>
+      </c>
       <c r="G204" t="s">
         <v>313</v>
       </c>
@@ -5049,6 +5357,9 @@
       <c r="C205" t="s">
         <v>2</v>
       </c>
+      <c r="D205" t="s">
+        <v>476</v>
+      </c>
       <c r="G205" t="s">
         <v>313</v>
       </c>
@@ -5063,6 +5374,9 @@
       <c r="C206" t="s">
         <v>2</v>
       </c>
+      <c r="D206" t="s">
+        <v>475</v>
+      </c>
       <c r="G206" t="s">
         <v>313</v>
       </c>
@@ -5078,10 +5392,10 @@
         <v>2</v>
       </c>
       <c r="D207" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E207" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G207" t="s">
         <v>313</v>
@@ -5097,6 +5411,9 @@
       <c r="C208" t="s">
         <v>2</v>
       </c>
+      <c r="D208" t="s">
+        <v>477</v>
+      </c>
       <c r="G208" t="s">
         <v>313</v>
       </c>
@@ -5272,7 +5589,7 @@
         <v>2</v>
       </c>
       <c r="D223" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -5285,6 +5602,9 @@
       <c r="C224" t="s">
         <v>2</v>
       </c>
+      <c r="D224" t="s">
+        <v>478</v>
+      </c>
       <c r="G224" t="s">
         <v>313</v>
       </c>
@@ -5328,7 +5648,7 @@
         <v>2</v>
       </c>
       <c r="D227" t="s">
-        <v>426</v>
+        <v>479</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -5341,6 +5661,9 @@
       <c r="C228" t="s">
         <v>2</v>
       </c>
+      <c r="D228" t="s">
+        <v>480</v>
+      </c>
       <c r="G228" t="s">
         <v>313</v>
       </c>
@@ -5441,6 +5764,9 @@
       <c r="C236" t="s">
         <v>2</v>
       </c>
+      <c r="D236" t="s">
+        <v>481</v>
+      </c>
       <c r="G236" t="s">
         <v>313</v>
       </c>
@@ -5477,6 +5803,9 @@
       <c r="C239" t="s">
         <v>2</v>
       </c>
+      <c r="D239" t="s">
+        <v>482</v>
+      </c>
       <c r="G239" t="s">
         <v>313</v>
       </c>
@@ -5506,7 +5835,7 @@
         <v>2</v>
       </c>
       <c r="D241" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -5577,6 +5906,9 @@
       <c r="C247" t="s">
         <v>2</v>
       </c>
+      <c r="D247" t="s">
+        <v>483</v>
+      </c>
       <c r="G247" t="s">
         <v>313</v>
       </c>
@@ -5624,6 +5956,9 @@
       <c r="C251" t="s">
         <v>2</v>
       </c>
+      <c r="D251" t="s">
+        <v>484</v>
+      </c>
       <c r="G251" t="s">
         <v>313</v>
       </c>
@@ -5638,9 +5973,6 @@
       <c r="C252" t="s">
         <v>2</v>
       </c>
-      <c r="D252" t="s">
-        <v>417</v>
-      </c>
       <c r="I252" t="s">
         <v>313</v>
       </c>
@@ -5654,9 +5986,6 @@
       </c>
       <c r="C253" t="s">
         <v>2</v>
-      </c>
-      <c r="D253" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
@@ -49156,19 +49485,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B1" t="s">
         <v>368</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1" t="s">
         <v>369</v>
       </c>
-      <c r="C1" t="s">
-        <v>405</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>370</v>
-      </c>
-      <c r="E1" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -49176,7 +49505,7 @@
         <v>331</v>
       </c>
       <c r="B2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -49187,10 +49516,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -49215,7 +49544,7 @@
         <v>334</v>
       </c>
       <c r="B5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -49229,7 +49558,7 @@
         <v>335</v>
       </c>
       <c r="B6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -49243,7 +49572,7 @@
         <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -49257,7 +49586,7 @@
         <v>355</v>
       </c>
       <c r="B8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -49271,7 +49600,7 @@
         <v>337</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -49285,10 +49614,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -49302,7 +49631,7 @@
         <v>341</v>
       </c>
       <c r="C11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -49316,7 +49645,7 @@
         <v>338</v>
       </c>
       <c r="C12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -49330,7 +49659,7 @@
         <v>342</v>
       </c>
       <c r="B13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -49344,7 +49673,7 @@
         <v>343</v>
       </c>
       <c r="B14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -49358,7 +49687,7 @@
         <v>344</v>
       </c>
       <c r="B15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
@@ -49372,10 +49701,10 @@
         <v>345</v>
       </c>
       <c r="B16" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
@@ -49400,10 +49729,10 @@
         <v>311</v>
       </c>
       <c r="B18" t="s">
+        <v>393</v>
+      </c>
+      <c r="C18" t="s">
         <v>394</v>
-      </c>
-      <c r="C18" t="s">
-        <v>395</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
@@ -49428,7 +49757,7 @@
         <v>347</v>
       </c>
       <c r="B20" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -49442,10 +49771,10 @@
         <v>348</v>
       </c>
       <c r="B21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -49459,7 +49788,7 @@
         <v>349</v>
       </c>
       <c r="B22" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D22" t="s">
         <v>46</v>
@@ -49473,7 +49802,7 @@
         <v>350</v>
       </c>
       <c r="B23" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D23" t="s">
         <v>46</v>
@@ -49487,7 +49816,7 @@
         <v>351</v>
       </c>
       <c r="B24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
@@ -49512,7 +49841,7 @@
         <v>353</v>
       </c>
       <c r="B26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D26" t="s">
         <v>46</v>
@@ -49526,7 +49855,7 @@
         <v>357</v>
       </c>
       <c r="C27" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D27" t="s">
         <v>46</v>
@@ -49540,7 +49869,7 @@
         <v>359</v>
       </c>
       <c r="B28" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D28" t="s">
         <v>46</v>
@@ -49551,10 +49880,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D29" t="s">
         <v>46</v>
@@ -49565,10 +49894,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>384</v>
+      </c>
+      <c r="B30" t="s">
         <v>385</v>
-      </c>
-      <c r="B30" t="s">
-        <v>386</v>
       </c>
       <c r="D30" t="s">
         <v>46</v>
@@ -49579,13 +49908,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B31" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C31" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D31" t="s">
         <v>46</v>
@@ -49609,7 +49938,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Steve's update of spreadsheet
</commit_message>
<xml_diff>
--- a/testing/Variables with types.xlsx
+++ b/testing/Variables with types.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13019" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13020" uniqueCount="486">
   <si>
     <t>A_Global</t>
   </si>
@@ -1531,6 +1531,9 @@
   <si>
     <t>total_AP_prodn_shortfall</t>
   </si>
+  <si>
+    <t>CP_protein_content</t>
+  </si>
 </sst>
 </file>
 
@@ -2360,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K82" sqref="K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4063,6 +4066,9 @@
       </c>
       <c r="C112" t="s">
         <v>2</v>
+      </c>
+      <c r="D112" t="s">
+        <v>485</v>
       </c>
       <c r="G112" t="s">
         <v>313</v>

</xml_diff>

<commit_message>
completes definition column in tab 2
</commit_message>
<xml_diff>
--- a/testing/Variables with types.xlsx
+++ b/testing/Variables with types.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13010" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13018" uniqueCount="494">
   <si>
     <t>A_Global</t>
   </si>
@@ -1534,6 +1534,30 @@
   <si>
     <t>commodity product</t>
   </si>
+  <si>
+    <t>modification</t>
+  </si>
+  <si>
+    <t>Animal Product Production Shortfall</t>
+  </si>
+  <si>
+    <t>Commodity product Production Shortfall</t>
+  </si>
+  <si>
+    <t>commodity</t>
+  </si>
+  <si>
+    <t>Commodity</t>
+  </si>
+  <si>
+    <t>Forage</t>
+  </si>
+  <si>
+    <t>impact</t>
+  </si>
+  <si>
+    <t>NOTE THAT THE EXAMPLE IS NO LONGER IN THE MODEL</t>
+  </si>
 </sst>
 </file>
 
@@ -49438,10 +49462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49502,6 +49526,9 @@
       <c r="A4" t="s">
         <v>353</v>
       </c>
+      <c r="B4" t="s">
+        <v>486</v>
+      </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -49600,6 +49627,9 @@
       <c r="A11" t="s">
         <v>339</v>
       </c>
+      <c r="B11" t="s">
+        <v>487</v>
+      </c>
       <c r="C11" t="s">
         <v>390</v>
       </c>
@@ -49614,6 +49644,9 @@
       <c r="A12" t="s">
         <v>336</v>
       </c>
+      <c r="B12" t="s">
+        <v>488</v>
+      </c>
       <c r="C12" t="s">
         <v>390</v>
       </c>
@@ -49683,9 +49716,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>489</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
@@ -49694,7 +49730,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>311</v>
       </c>
@@ -49711,10 +49747,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>344</v>
       </c>
+      <c r="B19" t="s">
+        <v>490</v>
+      </c>
       <c r="D19" t="s">
         <v>46</v>
       </c>
@@ -49722,7 +49761,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>345</v>
       </c>
@@ -49736,7 +49775,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>346</v>
       </c>
@@ -49753,7 +49792,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>347</v>
       </c>
@@ -49767,7 +49806,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>348</v>
       </c>
@@ -49781,7 +49820,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>349</v>
       </c>
@@ -49795,10 +49834,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>350</v>
       </c>
+      <c r="B25" t="s">
+        <v>491</v>
+      </c>
       <c r="D25" t="s">
         <v>46</v>
       </c>
@@ -49806,7 +49848,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>351</v>
       </c>
@@ -49820,10 +49862,13 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>354</v>
       </c>
+      <c r="B27" t="s">
+        <v>492</v>
+      </c>
       <c r="C27" t="s">
         <v>397</v>
       </c>
@@ -49833,8 +49878,11 @@
       <c r="E27" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>356</v>
       </c>
@@ -49848,7 +49896,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>391</v>
       </c>
@@ -49862,7 +49910,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>381</v>
       </c>
@@ -49876,7 +49924,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>362</v>
       </c>

</xml_diff>